<commit_message>
Debug PY und AuroraAPI
debug GUI wurde weiterentwickelt.
Aufbau eine Aurora API zur abstrahierung der seriellen Schnittstelle
</commit_message>
<xml_diff>
--- a/doc/Uvis_19+20/Stundenprotokoll_Camed_Uvis.xlsx
+++ b/doc/Uvis_19+20/Stundenprotokoll_Camed_Uvis.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
   <si>
     <t>Projekte:</t>
   </si>
@@ -174,6 +174,21 @@
   </si>
   <si>
     <t>Restrukturierung der Doku + Einarbeitung mit neuem Teammitglied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Doku lesen und relevante Inhalt rausschreiben. </t>
+  </si>
+  <si>
+    <t>Debug GUI einrichten für Pyserial + Tkinter</t>
+  </si>
+  <si>
+    <t>Aurora API Schnittstellen ansprechen und Daten auslesen</t>
+  </si>
+  <si>
+    <t>Python Aurora API entwickeln</t>
+  </si>
+  <si>
+    <t>Studieninfotag - Betreuung der Teilnehmer</t>
   </si>
 </sst>
 </file>
@@ -869,7 +884,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -961,6 +976,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -991,10 +1007,31 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1033,44 +1070,14 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1078,19 +1085,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1100,30 +1102,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1146,16 +1124,54 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1282,73 +1298,7 @@
     <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1594,7 +1544,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1605,18 +1555,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1638,6 +1577,17 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="2" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
@@ -1649,7 +1599,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1804,18 +1754,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A6:G504" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A6:G504" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A6:G504"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Datum" dataDxfId="12"/>
-    <tableColumn id="2" name="Von" dataDxfId="11"/>
-    <tableColumn id="3" name="Bis" dataDxfId="10"/>
-    <tableColumn id="4" name="Arbeitszeit" dataDxfId="9">
+    <tableColumn id="1" name="Datum" dataDxfId="6"/>
+    <tableColumn id="2" name="Von" dataDxfId="5"/>
+    <tableColumn id="3" name="Bis" dataDxfId="4"/>
+    <tableColumn id="4" name="Arbeitszeit" dataDxfId="3">
       <calculatedColumnFormula>SUM(C7-B7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Projekt" dataDxfId="8"/>
-    <tableColumn id="6" name="Aufgabe" dataDxfId="7"/>
-    <tableColumn id="7" name="Beschreibung" dataDxfId="6"/>
+    <tableColumn id="5" name="Projekt" dataDxfId="2"/>
+    <tableColumn id="6" name="Aufgabe" dataDxfId="1"/>
+    <tableColumn id="7" name="Beschreibung" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2143,13 +2093,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J505"/>
+  <dimension ref="A1:N505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2161,57 +2111,62 @@
     <col min="8" max="8" width="10.796875" style="13"/>
     <col min="9" max="9" width="23.296875" style="13" customWidth="1"/>
     <col min="10" max="10" width="10.796875" style="13"/>
+    <col min="14" max="14" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="65"/>
+      <c r="N2" s="59">
+        <f ca="1">TODAY()</f>
+        <v>43790</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="25">
         <f>SUM(D7:D504)</f>
-        <v>0.93749999999999978</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
@@ -2220,19 +2175,19 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="68"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
         <v>32</v>
       </c>
@@ -2255,7 +2210,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="52">
         <v>43746</v>
       </c>
@@ -2279,7 +2234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="52">
         <v>43752</v>
       </c>
@@ -2303,7 +2258,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="52">
         <v>43753</v>
       </c>
@@ -2327,7 +2282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="53">
         <v>43760</v>
       </c>
@@ -2351,7 +2306,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="53">
         <v>43761</v>
       </c>
@@ -2375,7 +2330,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="53">
         <v>43768</v>
       </c>
@@ -2399,103 +2354,171 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="53">
+        <v>43769</v>
+      </c>
+      <c r="B13" s="55">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C13" s="55">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D13" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.2499999999999944E-2</v>
       </c>
       <c r="E13" s="56" t="s">
         <v>36</v>
       </c>
       <c r="F13" s="37"/>
-      <c r="G13" s="42"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
+      <c r="G13" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="59">
+        <v>43774</v>
+      </c>
+      <c r="B14" s="55">
+        <v>0.6875</v>
+      </c>
+      <c r="C14" s="55">
+        <v>0.8125</v>
+      </c>
       <c r="D14" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="E14" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="42"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="53"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
+      <c r="F14" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="53">
+        <v>43783</v>
+      </c>
+      <c r="B15" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="55">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="D15" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13541666666666663</v>
       </c>
       <c r="E15" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="42"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="53"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
+      <c r="F15" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="53">
+        <v>43788</v>
+      </c>
+      <c r="B16" s="55">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C16" s="55">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D16" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="42"/>
+      <c r="F16" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
+      <c r="A17" s="53">
+        <v>43789</v>
+      </c>
+      <c r="B17" s="55">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C17" s="55">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="D17" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28125000000000006</v>
       </c>
       <c r="E17" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="42"/>
+        <v>11</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="53"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
+      <c r="A18" s="53">
+        <v>43789</v>
+      </c>
+      <c r="B18" s="55">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C18" s="55">
+        <v>1</v>
+      </c>
       <c r="D18" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="E18" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="42"/>
+      <c r="F18" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="42" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="53"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
+      <c r="A19" s="53">
+        <v>43790</v>
+      </c>
+      <c r="B19" s="55">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C19" s="55">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D19" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333315E-2</v>
       </c>
       <c r="E19" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="42"/>
+      <c r="F19" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="53"/>
@@ -9773,7 +9796,7 @@
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="E505">
-    <cfRule type="containsText" dxfId="34" priority="2909" operator="containsText" text="Kinect">
+    <cfRule type="containsText" dxfId="28" priority="2909" operator="containsText" text="Kinect">
       <formula>NOT(ISERROR(SEARCH("Kinect",E505)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10100,20 +10123,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="D1" s="85" t="s">
+      <c r="B1" s="71"/>
+      <c r="D1" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="86"/>
+      <c r="E1" s="73"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="88"/>
-      <c r="B2" s="88"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
@@ -10122,7 +10145,7 @@
       </c>
       <c r="B3" s="26">
         <f>SUMIF(CaMed_Arbeitszeittabelle!$E:$E,A3,CaMed_Arbeitszeittabelle!$D:$D)</f>
-        <v>0.93749999999999978</v>
+        <v>1.5520833333333333</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>7</v>
@@ -10146,7 +10169,7 @@
       </c>
       <c r="E4" s="26">
         <f>SUMIF(CaMed_Arbeitszeittabelle!F:F,D4,CaMed_Arbeitszeittabelle!D:D)</f>
-        <v>0.74999999999999989</v>
+        <v>1.3020833333333333</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -10190,7 +10213,7 @@
       </c>
       <c r="B7" s="26">
         <f>SUMIF(CaMed_Arbeitszeittabelle!$E:$E,A7,CaMed_Arbeitszeittabelle!$D:$D)</f>
-        <v>0</v>
+        <v>0.28125000000000006</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>10</v>
@@ -10218,14 +10241,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
-      <c r="B9" s="70"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="77"/>
       <c r="D9" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="26">
         <f>SUMIF(CaMed_Arbeitszeittabelle!F:F,D9,CaMed_Arbeitszeittabelle!D:D)</f>
-        <v>0</v>
+        <v>0.28125000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -10234,7 +10257,7 @@
       </c>
       <c r="B10" s="51">
         <f>SUM(B3:B8)</f>
-        <v>0.93749999999999978</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>6</v>
@@ -10247,8 +10270,8 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" s="50"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="70"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="77"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="34"/>
@@ -10258,22 +10281,22 @@
       </c>
       <c r="E12" s="22">
         <f>SUM(E3:E10)</f>
-        <v>0.93749999999999978</v>
+        <v>1.7708333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="D14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="D14" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="82"/>
-      <c r="G14" s="75" t="s">
+      <c r="E14" s="90"/>
+      <c r="G14" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="76"/>
+      <c r="H14" s="84"/>
     </row>
     <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
@@ -10304,7 +10327,7 @@
       </c>
       <c r="B16" s="27">
         <f>SUMPRODUCT((CaMed_Arbeitszeittabelle!$E$7:$E$504=$A$14)*(CaMed_Arbeitszeittabelle!$F$7:$F$504=A16)*(CaMed_Arbeitszeittabelle!$D$7:$D$504))</f>
-        <v>0.74999999999999989</v>
+        <v>1.3020833333333333</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>4</v>
@@ -10465,7 +10488,7 @@
       </c>
       <c r="B23" s="28">
         <f>SUM(B15:B22)</f>
-        <v>0.93749999999999978</v>
+        <v>1.4895833333333333</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>12</v>
@@ -10483,19 +10506,19 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="72"/>
-      <c r="D26" s="73" t="s">
+      <c r="B26" s="80"/>
+      <c r="D26" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="74"/>
+      <c r="E26" s="82"/>
       <c r="F26" s="34"/>
-      <c r="G26" s="77" t="s">
+      <c r="G26" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="78"/>
+      <c r="H26" s="86"/>
     </row>
     <row r="27" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" s="23" t="s">
@@ -10654,7 +10677,7 @@
       </c>
       <c r="E33" s="27">
         <f>SUMPRODUCT((CaMed_Arbeitszeittabelle!$E$7:$E$504=$D$26)*(CaMed_Arbeitszeittabelle!$F$7:$F$504=D33)*(CaMed_Arbeitszeittabelle!$D$7:$D$504))</f>
-        <v>0</v>
+        <v>0.28125000000000006</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="6" t="s">
@@ -10702,7 +10725,7 @@
       </c>
       <c r="E35" s="28">
         <f>SUM(E27:E34)</f>
-        <v>0</v>
+        <v>0.28125000000000006</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="18" t="s">
@@ -10715,11 +10738,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:B9"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="D26:E26"/>
@@ -10727,6 +10745,11 @@
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -10752,349 +10775,349 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="119"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="104"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="104"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="106"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="101"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
       <c r="D3" s="34"/>
-      <c r="E3" s="120" t="s">
+      <c r="E3" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="120"/>
-      <c r="G3" s="121"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="106"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
       <c r="D4" s="34"/>
-      <c r="E4" s="120">
+      <c r="E4" s="105">
         <v>766641</v>
       </c>
-      <c r="F4" s="120"/>
-      <c r="G4" s="121"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="106"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="123"/>
-      <c r="C5" s="123"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
       <c r="D5" s="34"/>
-      <c r="E5" s="120" t="s">
+      <c r="E5" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="120"/>
-      <c r="G5" s="121"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="106"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="104"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="101"/>
     </row>
     <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="126"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="93"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="97"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
       <c r="D8" s="29"/>
-      <c r="E8" s="127">
+      <c r="E8" s="96">
         <f>Gesamtstundenübersicht!$B$10</f>
-        <v>0.93749999999999978</v>
-      </c>
-      <c r="F8" s="92"/>
-      <c r="G8" s="93"/>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="F8" s="97"/>
+      <c r="G8" s="98"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="104"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="106"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="101"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="110"/>
       <c r="D10" s="30"/>
-      <c r="E10" s="107" t="s">
+      <c r="E10" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="107"/>
-      <c r="G10" s="108"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="112"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="96" t="str">
+      <c r="A11" s="94" t="str">
         <f>Gesamtstundenübersicht!A3</f>
         <v>CaMed allgemein</v>
       </c>
-      <c r="B11" s="97"/>
-      <c r="C11" s="97"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="29"/>
-      <c r="E11" s="92">
+      <c r="E11" s="97">
         <f>Gesamtstundenübersicht!B3</f>
-        <v>0.93749999999999978</v>
-      </c>
-      <c r="F11" s="92"/>
-      <c r="G11" s="93"/>
+        <v>1.5520833333333333</v>
+      </c>
+      <c r="F11" s="97"/>
+      <c r="G11" s="98"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="96" t="str">
+      <c r="A12" s="94" t="str">
         <f>Gesamtstundenübersicht!A4</f>
         <v>Projektmanagement</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="29"/>
-      <c r="E12" s="92">
+      <c r="E12" s="97">
         <f>Gesamtstundenübersicht!B4</f>
         <v>0</v>
       </c>
-      <c r="F12" s="92"/>
-      <c r="G12" s="93"/>
+      <c r="F12" s="97"/>
+      <c r="G12" s="98"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="96" t="str">
+      <c r="A13" s="94" t="str">
         <f>Gesamtstundenübersicht!A5</f>
         <v>Öffentlichkeitsarbeit</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="92">
+      <c r="E13" s="97">
         <f>Gesamtstundenübersicht!B5</f>
         <v>0</v>
       </c>
-      <c r="F13" s="92"/>
-      <c r="G13" s="93"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="98"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="96" t="str">
+      <c r="A14" s="94" t="str">
         <f>Gesamtstundenübersicht!A6</f>
         <v>Infrastruktur</v>
       </c>
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
       <c r="D14" s="29"/>
-      <c r="E14" s="92">
+      <c r="E14" s="97">
         <f>Gesamtstundenübersicht!B6</f>
         <v>0</v>
       </c>
-      <c r="F14" s="92"/>
-      <c r="G14" s="93"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="98"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="96" t="str">
+      <c r="A15" s="94" t="str">
         <f>Gesamtstundenübersicht!A7</f>
         <v>Veranstaltungen</v>
       </c>
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="29"/>
-      <c r="E15" s="92">
+      <c r="E15" s="97">
         <f>Gesamtstundenübersicht!B7</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="92"/>
-      <c r="G15" s="93"/>
+        <v>0.28125000000000006</v>
+      </c>
+      <c r="F15" s="97"/>
+      <c r="G15" s="98"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="96" t="str">
+      <c r="A16" s="94" t="str">
         <f>Gesamtstundenübersicht!A8</f>
         <v>Middleware Projekt</v>
       </c>
-      <c r="B16" s="97"/>
-      <c r="C16" s="97"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
       <c r="D16" s="29"/>
-      <c r="E16" s="92">
+      <c r="E16" s="97">
         <f>Gesamtstundenübersicht!B8</f>
         <v>0</v>
       </c>
-      <c r="F16" s="92"/>
-      <c r="G16" s="93"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="98"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="104"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="106"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="101"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="102"/>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="103"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="126"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="90" t="str">
+      <c r="A19" s="116" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D3)</f>
         <v>davon Dokumentation</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="117"/>
       <c r="D19" s="29"/>
-      <c r="E19" s="92">
+      <c r="E19" s="97">
         <f>Gesamtstundenübersicht!E3</f>
         <v>0.18749999999999994</v>
       </c>
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="98"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="90" t="str">
+      <c r="A20" s="116" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D4)</f>
         <v>davon Einarbeitung</v>
       </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="117"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="92">
+      <c r="E20" s="97">
         <f>Gesamtstundenübersicht!E4</f>
-        <v>0.74999999999999989</v>
-      </c>
-      <c r="F20" s="92"/>
-      <c r="G20" s="93"/>
+        <v>1.3020833333333333</v>
+      </c>
+      <c r="F20" s="97"/>
+      <c r="G20" s="98"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="90" t="str">
+      <c r="A21" s="116" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D5)</f>
         <v>davon Konzeption</v>
       </c>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
+      <c r="B21" s="117"/>
+      <c r="C21" s="117"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="92">
+      <c r="E21" s="97">
         <f>Gesamtstundenübersicht!E5</f>
         <v>0</v>
       </c>
-      <c r="F21" s="92"/>
-      <c r="G21" s="93"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="98"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="90" t="str">
+      <c r="A22" s="116" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D6)</f>
         <v>davon Meeting</v>
       </c>
-      <c r="B22" s="91"/>
-      <c r="C22" s="91"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="117"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="92">
+      <c r="E22" s="97">
         <f>Gesamtstundenübersicht!E6</f>
         <v>0</v>
       </c>
-      <c r="F22" s="92"/>
-      <c r="G22" s="93"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="98"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="90" t="str">
+      <c r="A23" s="116" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D7)</f>
         <v>davon Präsentation</v>
       </c>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="92">
+      <c r="E23" s="97">
         <f>Gesamtstundenübersicht!E7</f>
         <v>0</v>
       </c>
-      <c r="F23" s="92"/>
-      <c r="G23" s="93"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="98"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="90" t="str">
+      <c r="A24" s="116" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D8)</f>
         <v>davon Projektmanagement</v>
       </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="117"/>
       <c r="D24" s="38"/>
-      <c r="E24" s="92">
+      <c r="E24" s="97">
         <f>Gesamtstundenübersicht!E8</f>
         <v>0</v>
       </c>
-      <c r="F24" s="92"/>
-      <c r="G24" s="93"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="98"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="90" t="str">
+      <c r="A25" s="116" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D9)</f>
         <v>davon Sonstiges</v>
       </c>
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="117"/>
       <c r="D25" s="38"/>
-      <c r="E25" s="92">
+      <c r="E25" s="97">
         <f>Gesamtstundenübersicht!E9</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="92"/>
-      <c r="G25" s="93"/>
+        <v>0.28125000000000006</v>
+      </c>
+      <c r="F25" s="97"/>
+      <c r="G25" s="98"/>
     </row>
     <row r="26" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="115" t="str">
+      <c r="A26" s="121" t="str">
         <f>CONCATENATE("davon ",Gesamtstundenübersicht!D10)</f>
         <v>davon Umsetzung</v>
       </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
       <c r="D26" s="31"/>
-      <c r="E26" s="94">
+      <c r="E26" s="127">
         <f>Gesamtstundenübersicht!E10</f>
         <v>0</v>
       </c>
-      <c r="F26" s="94"/>
-      <c r="G26" s="95"/>
+      <c r="F26" s="127"/>
+      <c r="G26" s="128"/>
     </row>
     <row r="27" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="33"/>
@@ -11106,53 +11129,61 @@
       <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="112" t="s">
+      <c r="A28" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="113"/>
-      <c r="G28" s="114"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
+      <c r="G28" s="120"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="98" t="s">
+      <c r="A29" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="97"/>
-      <c r="C29" s="97"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
       <c r="D29" s="29"/>
-      <c r="E29" s="99" t="s">
+      <c r="E29" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="99"/>
-      <c r="G29" s="100"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="125"/>
     </row>
     <row r="30" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="109"/>
-      <c r="B30" s="110"/>
-      <c r="C30" s="110"/>
+      <c r="A30" s="113"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
       <c r="D30" s="32"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="110"/>
-      <c r="G30" s="111"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="A30:C30"/>
@@ -11169,27 +11200,19 @@
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A6:G6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>